<commit_message>
docs():Improve report per suggestions by reviewer
</commit_message>
<xml_diff>
--- a/capstone_project_charts.xlsx
+++ b/capstone_project_charts.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KNN Classifier n=1" sheetId="1" r:id="rId1"/>
+    <sheet name="Decision Tree" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="8">
   <si>
     <t>Samples</t>
   </si>
@@ -386,11 +387,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2116600480"/>
-        <c:axId val="-2122341744"/>
+        <c:axId val="2111252912"/>
+        <c:axId val="2111256240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2116600480"/>
+        <c:axId val="2111252912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -447,12 +448,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122341744"/>
+        <c:crossAx val="2111256240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122341744"/>
+        <c:axId val="2111256240"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -510,7 +511,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2116600480"/>
+        <c:crossAx val="2111252912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1415,8 +1416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1608,4 +1609,192 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>100000</v>
+      </c>
+      <c r="B3">
+        <v>391.23500000000001</v>
+      </c>
+      <c r="C3" s="1" t="e">
+        <f>B3/B2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D3">
+        <v>16.181000000000001</v>
+      </c>
+      <c r="E3" s="1" t="e">
+        <f>D3/D2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F6" si="0">D3/B3</f>
+        <v>4.1358774138305625E-2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>15.515000000000001</v>
+      </c>
+      <c r="H3" s="1" t="e">
+        <f>G3/G2</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1000000</v>
+      </c>
+      <c r="B4">
+        <v>11.641999999999999</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:C6" si="1">B4/B3</f>
+        <v>2.9757051388551635E-2</v>
+      </c>
+      <c r="D4">
+        <v>345.17500000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E6" si="2">D4/D3</f>
+        <v>21.332117916074409</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>29.649115272289986</v>
+      </c>
+      <c r="G4" s="2">
+        <f>0.1439*100</f>
+        <v>14.39</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H6" si="3">G4/G3</f>
+        <v>0.92748952626490488</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2000000</v>
+      </c>
+      <c r="B5">
+        <v>74.216999999999999</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="1"/>
+        <v>6.3749355780793682</v>
+      </c>
+      <c r="D5">
+        <v>942.86800000000005</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="2"/>
+        <v>2.7315651481132761</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>12.704205235997144</v>
+      </c>
+      <c r="G5" s="2">
+        <v>21.36</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="3"/>
+        <v>1.4843641417651146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5000000</v>
+      </c>
+      <c r="B6">
+        <v>554.94100000000003</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="1"/>
+        <v>7.4772760957732061</v>
+      </c>
+      <c r="D6">
+        <v>3184.24</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="2"/>
+        <v>3.3771853536232004</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>5.7379793527600222</v>
+      </c>
+      <c r="G6" s="2">
+        <v>30.49</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="3"/>
+        <v>1.4274344569288389</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
docs(): Revise per review
</commit_message>
<xml_diff>
--- a/capstone_project_charts.xlsx
+++ b/capstone_project_charts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KNN Classifier n=1" sheetId="1" r:id="rId1"/>
     <sheet name="Decision Tree" sheetId="2" r:id="rId2"/>
+    <sheet name="Final Solution Comparison" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
   <si>
     <t>Samples</t>
   </si>
@@ -53,13 +54,29 @@
   <si>
     <t>Score Improvement %</t>
   </si>
+  <si>
+    <t>Composite Solution</t>
+  </si>
+  <si>
+    <t>1-NN 10,000</t>
+  </si>
+  <si>
+    <t>1-NN 5,000,000</t>
+  </si>
+  <si>
+    <t>Training Time (Seconds)</t>
+  </si>
+  <si>
+    <t>Accuracy Score (%)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -99,10 +116,11 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -387,11 +405,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2111252912"/>
-        <c:axId val="2111256240"/>
+        <c:axId val="-2110124816"/>
+        <c:axId val="-2110121552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2111252912"/>
+        <c:axId val="-2110124816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -448,12 +466,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2111256240"/>
+        <c:crossAx val="-2110121552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2111256240"/>
+        <c:axId val="-2110121552"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -511,7 +529,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2111252912"/>
+        <c:crossAx val="-2110124816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -560,7 +578,573 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Final Method, Baseline Comparison</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Final Solution Comparison'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Training Time (Seconds)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Final Solution Comparison'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1-NN 10,000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1-NN 5,000,000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Composite Solution</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Final Solution Comparison'!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>554.941</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1706</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Final Solution Comparison'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy Score (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Final Solution Comparison'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1-NN 10,000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1-NN 5,000,000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Composite Solution</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Final Solution Comparison'!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.0000_);_(* \(#,##0.0000\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59.68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="-2107975984"/>
+        <c:axId val="-2107941536"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2107975984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2107941536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2107941536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2107975984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1116,6 +1700,511 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1149,6 +2238,78 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.85498</cdr:x>
+      <cdr:y>0.52113</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.96375</cdr:x>
+      <cdr:y>0.72394</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7188200" y="2349500"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1417,7 +2578,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1615,7 +2776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -1797,4 +2958,69 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C2" s="3">
+        <f>0.009*100</f>
+        <v>0.89999999999999991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>554.94100000000003</v>
+      </c>
+      <c r="C3" s="3">
+        <f>0.3049*100</f>
+        <v>30.490000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>0.1706</v>
+      </c>
+      <c r="C4" s="3">
+        <f>0.5968*100</f>
+        <v>59.68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>